<commit_message>
edit docs from 3.2
</commit_message>
<xml_diff>
--- a/docs/resources/SourceDictionary.xlsx
+++ b/docs/resources/SourceDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84F17B0-40CF-4E48-987E-BE54B14B0022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B758037-76EA-479B-9446-A0CCD1C1237A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -431,7 +431,7 @@
     <col min="4" max="4" width="22.25" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.8125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1875" style="7" customWidth="1"/>
     <col min="8" max="28" width="7.6875" style="7" customWidth="1"/>
     <col min="29" max="16384" width="12.6875" style="7"/>
   </cols>
@@ -3744,7 +3744,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3760,10 +3760,12 @@
     <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.0625" bestFit="1" customWidth="1"/>
-    <col min="9" max="27" width="7.6875" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.8125" bestFit="1" customWidth="1"/>
+    <col min="11" max="27" width="7.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -3788,8 +3790,14 @@
       <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="I1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
@@ -3799,7 +3807,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
@@ -3809,7 +3817,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
@@ -3819,7 +3827,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
@@ -3829,7 +3837,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
@@ -3839,7 +3847,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>
@@ -3849,7 +3857,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
@@ -3859,7 +3867,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
@@ -3869,7 +3877,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
@@ -3879,7 +3887,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
@@ -3889,17 +3897,17 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update templates and docs
</commit_message>
<xml_diff>
--- a/docs/resources/SourceDictionary.xlsx
+++ b/docs/resources/SourceDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A97435-374F-4DC2-8859-313F739459C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA982BD1-5197-484D-AC01-18C73028E823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -99,12 +99,6 @@
     <t>is repeat of.name</t>
   </si>
   <si>
-    <t>collection event.resource</t>
-  </si>
-  <si>
-    <t>collection event.name</t>
-  </si>
-  <si>
     <t>is repeat of.dataset</t>
   </si>
   <si>
@@ -112,6 +106,9 @@
   </si>
   <si>
     <t>variable.name</t>
+  </si>
+  <si>
+    <t>collection event</t>
   </si>
 </sst>
 </file>
@@ -420,7 +417,7 @@
   <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1475,9 +1472,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S1003"/>
+  <dimension ref="A1:R1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1489,22 +1488,21 @@
     <col min="6" max="6" width="8.625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.0625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.1875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.8125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="28" width="7.6875" style="5" customWidth="1"/>
-    <col min="29" max="16384" width="12.6875" style="5"/>
+    <col min="9" max="9" width="12.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.8125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="27" width="7.6875" style="5" customWidth="1"/>
+    <col min="28" max="16384" width="12.6875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1530,40 +1528,37 @@
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="5"/>
       <c r="D2" s="4"/>
@@ -1573,94 +1568,90 @@
       <c r="H2" s="4"/>
       <c r="I2" s="7"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="R2" s="8"/>
+      <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="5"/>
       <c r="E3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="4"/>
-      <c r="R3" s="8"/>
+      <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="5"/>
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="4"/>
-      <c r="R4" s="8"/>
+      <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="5"/>
       <c r="H5" s="4"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="5"/>
       <c r="G7" s="6"/>
       <c r="H7" s="4"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="5"/>
       <c r="G9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="7"/>
-      <c r="R13" s="8"/>
+      <c r="Q13" s="8"/>
     </row>
-    <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="5"/>
       <c r="E14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2682,10 +2673,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -3748,7 +3739,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3762,14 +3753,13 @@
     <col min="4" max="4" width="4.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.0625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.8125" bestFit="1" customWidth="1"/>
-    <col min="11" max="27" width="7.6875" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="7.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -3783,25 +3773,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
+      <c r="H1" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
@@ -3809,9 +3796,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
@@ -3819,9 +3805,8 @@
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
@@ -3829,9 +3814,8 @@
       <c r="E4" s="3"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
@@ -3839,9 +3823,8 @@
       <c r="E5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="5"/>
@@ -3849,9 +3832,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>
@@ -3859,9 +3841,8 @@
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
@@ -3869,9 +3850,8 @@
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
@@ -3879,9 +3859,8 @@
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
@@ -3889,9 +3868,8 @@
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
@@ -3899,19 +3877,18 @@
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat: ema update (#2745)
* ontology and datamodel edits

* ema datamodel to separate folder for now

* Publications back to format of >=3.7
</commit_message>
<xml_diff>
--- a/docs/resources/SourceDictionary.xlsx
+++ b/docs/resources/SourceDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Molgenis\repos\molgenis-emx2\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A97435-374F-4DC2-8859-313F739459C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A9D396-C935-4F13-B6DA-74A886460E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,12 +99,6 @@
     <t>is repeat of.name</t>
   </si>
   <si>
-    <t>collection event.resource</t>
-  </si>
-  <si>
-    <t>collection event.name</t>
-  </si>
-  <si>
     <t>is repeat of.dataset</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>variable.name</t>
+  </si>
+  <si>
+    <t>collection event.resource</t>
+  </si>
+  <si>
+    <t>collection event.name</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1477,7 +1477,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="I1:J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1490,7 +1492,7 @@
     <col min="7" max="7" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.25" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.0625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.25" style="5" customWidth="1"/>
     <col min="11" max="11" width="36.75" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.25" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.1875" style="5" bestFit="1" customWidth="1"/>
@@ -1530,10 +1532,10 @@
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>2</v>
@@ -1572,7 +1574,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="4"/>
       <c r="R2" s="8"/>
     </row>
@@ -1582,7 +1584,7 @@
       <c r="E3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="7"/>
       <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1591,7 +1593,7 @@
       <c r="E4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="7"/>
       <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1599,12 +1601,14 @@
       <c r="B5" s="5"/>
       <c r="H5" s="4"/>
       <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="7"/>
       <c r="B6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7"/>
@@ -1612,12 +1616,14 @@
       <c r="G7" s="6"/>
       <c r="H7" s="4"/>
       <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="B8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="7"/>
@@ -1625,30 +1631,35 @@
       <c r="G9" s="6"/>
       <c r="H9" s="4"/>
       <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="7"/>
       <c r="B10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="R13" s="8"/>
     </row>
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1657,7 +1668,7 @@
       <c r="E14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2682,10 +2693,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -3783,16 +3794,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
+      <c r="G1" s="7" t="s">
+        <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>15</v>

</xml_diff>